<commit_message>
more data sets with duplicates
</commit_message>
<xml_diff>
--- a/data2-swap.xlsx
+++ b/data2-swap.xlsx
@@ -377,22 +377,22 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>5</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -403,74 +403,74 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -481,22 +481,22 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E6">
         <v>4</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -507,16 +507,16 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C7">
         <v>3</v>
       </c>
       <c r="D7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -528,33 +528,33 @@
         <v>1</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -562,51 +562,51 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H9">
         <v>2</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F10">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H10">
         <v>2</v>
       </c>
       <c r="J10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -614,71 +614,71 @@
         <v>6</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H11">
         <v>2</v>
       </c>
       <c r="J11">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H12">
         <v>2</v>
       </c>
       <c r="J12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D13">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H13">
         <v>2</v>
@@ -689,22 +689,22 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F14">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H14">
         <v>2</v>
@@ -715,22 +715,22 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F15">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H15">
         <v>2</v>
@@ -741,22 +741,22 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B16">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C16">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D16">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F16">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H16">
         <v>2</v>
@@ -767,22 +767,22 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D17">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E17">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H17">
         <v>2</v>
@@ -793,22 +793,22 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D18">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E18">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H18">
         <v>2</v>
@@ -819,22 +819,22 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B19">
         <v>4</v>
       </c>
       <c r="C19">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E19">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H19">
         <v>2</v>
@@ -845,100 +845,100 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B20">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D20">
         <v>5</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H20">
         <v>2</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B21">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C21">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F21">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H21">
         <v>2</v>
       </c>
       <c r="J21">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B22">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F22">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H22">
         <v>2</v>
       </c>
       <c r="J22">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B23">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C23">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E23">
         <v>3</v>
       </c>
       <c r="F23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H23">
         <v>2</v>
@@ -949,74 +949,74 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B24">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C24">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D24">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H24">
         <v>2</v>
       </c>
       <c r="J24">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B25">
         <v>2</v>
       </c>
       <c r="C25">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D25">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F25">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H25">
         <v>2</v>
       </c>
       <c r="J25">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B26">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C26">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H26">
         <v>2</v>
@@ -1027,126 +1027,126 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B27">
         <v>6</v>
       </c>
       <c r="C27">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D27">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E27">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F27">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H27">
         <v>3</v>
       </c>
       <c r="J27">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B28">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D28">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E28">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F28">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H28">
         <v>3</v>
       </c>
       <c r="J28">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B29">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C29">
         <v>3</v>
       </c>
       <c r="D29">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F29">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H29">
         <v>3</v>
       </c>
       <c r="J29">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B30">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D30">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E30">
         <v>3</v>
       </c>
       <c r="F30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H30">
         <v>3</v>
       </c>
       <c r="J30">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B31">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C31">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D31">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E31">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H31">
         <v>3</v>
@@ -1157,16 +1157,16 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B32">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C32">
         <v>3</v>
       </c>
       <c r="D32">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E32">
         <v>2</v>
@@ -1189,68 +1189,68 @@
         <v>6</v>
       </c>
       <c r="C33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D33">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E33">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F33">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H33">
         <v>3</v>
       </c>
       <c r="J33">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B34">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C34">
         <v>3</v>
       </c>
       <c r="D34">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E34">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F34">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H34">
         <v>3</v>
       </c>
       <c r="J34">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B35">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C35">
         <v>4</v>
       </c>
       <c r="D35">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E35">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F35">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H35">
         <v>3</v>
@@ -1261,22 +1261,22 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B36">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C36">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D36">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E36">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F36">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H36">
         <v>3</v>
@@ -1287,22 +1287,22 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C37">
         <v>3</v>
       </c>
       <c r="D37">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E37">
         <v>6</v>
       </c>
       <c r="F37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H37">
         <v>3</v>
@@ -1313,48 +1313,48 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B38">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C38">
         <v>3</v>
       </c>
       <c r="D38">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E38">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H38">
         <v>3</v>
       </c>
       <c r="J38">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D39">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E39">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H39">
         <v>3</v>
@@ -1365,22 +1365,22 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B40">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C40">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D40">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E40">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F40">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H40">
         <v>3</v>
@@ -1391,54 +1391,54 @@
     </row>
     <row r="41" spans="1:10">
       <c r="A41">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B41">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C41">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D41">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E41">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F41">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H41">
         <v>3</v>
       </c>
       <c r="J41">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C42">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D42">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E42">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H42">
         <v>4</v>
       </c>
       <c r="J42">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -1446,51 +1446,51 @@
         <v>6</v>
       </c>
       <c r="B43">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C43">
         <v>3</v>
       </c>
       <c r="D43">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H43">
         <v>4</v>
       </c>
       <c r="J43">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:10">
       <c r="A44">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B44">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C44">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D44">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E44">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F44">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H44">
         <v>4</v>
       </c>
       <c r="J44">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -1501,16 +1501,16 @@
         <v>6</v>
       </c>
       <c r="C45">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D45">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E45">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F45">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H45">
         <v>4</v>
@@ -1521,80 +1521,80 @@
     </row>
     <row r="46" spans="1:10">
       <c r="A46">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B46">
         <v>2</v>
       </c>
       <c r="C46">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D46">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E46">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F46">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H46">
         <v>4</v>
       </c>
       <c r="J46">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:10">
       <c r="A47">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B47">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C47">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D47">
         <v>5</v>
       </c>
       <c r="E47">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H47">
         <v>4</v>
       </c>
       <c r="J47">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:10">
       <c r="A48">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B48">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C48">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D48">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E48">
         <v>4</v>
       </c>
       <c r="F48">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H48">
         <v>4</v>
       </c>
       <c r="J48">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -1608,65 +1608,65 @@
         <v>3</v>
       </c>
       <c r="D49">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E49">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F49">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H49">
         <v>4</v>
       </c>
       <c r="J49">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C50">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D50">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E50">
         <v>6</v>
       </c>
       <c r="F50">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H50">
         <v>5</v>
       </c>
       <c r="J50">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:10">
       <c r="A51">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B51">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C51">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D51">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E51">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H51">
         <v>5</v>
@@ -1682,7 +1682,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L51"/>
+  <dimension ref="A1:L45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1704,22 +1704,22 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>5</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -1733,28 +1733,28 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -1762,28 +1762,28 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4">
         <v>1</v>
@@ -1791,22 +1791,22 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -1820,22 +1820,22 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E6">
         <v>4</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -1849,16 +1849,16 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C7">
         <v>3</v>
       </c>
       <c r="D7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -1870,7 +1870,7 @@
         <v>1</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L7">
         <v>1</v>
@@ -1878,28 +1878,28 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8">
         <v>1</v>
@@ -1910,25 +1910,25 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H9">
         <v>2</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9">
         <v>1</v>
@@ -1936,28 +1936,28 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F10">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H10">
         <v>2</v>
       </c>
       <c r="J10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L10">
         <v>1</v>
@@ -1968,25 +1968,25 @@
         <v>6</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H11">
         <v>2</v>
       </c>
       <c r="J11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L11">
         <v>1</v>
@@ -1994,51 +1994,51 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H12">
         <v>2</v>
       </c>
       <c r="J12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L12">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D13">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H13">
         <v>2</v>
@@ -2052,22 +2052,22 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F14">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H14">
         <v>2</v>
@@ -2076,27 +2076,27 @@
         <v>0</v>
       </c>
       <c r="L14">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F15">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H15">
         <v>2</v>
@@ -2105,27 +2105,27 @@
         <v>0</v>
       </c>
       <c r="L15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B16">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C16">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D16">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F16">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H16">
         <v>2</v>
@@ -2139,22 +2139,22 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D17">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E17">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H17">
         <v>2</v>
@@ -2168,22 +2168,22 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D18">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E18">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H18">
         <v>2</v>
@@ -2192,27 +2192,27 @@
         <v>1</v>
       </c>
       <c r="L18">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B19">
         <v>4</v>
       </c>
       <c r="C19">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E19">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H19">
         <v>2</v>
@@ -2226,57 +2226,57 @@
     </row>
     <row r="20" spans="1:12">
       <c r="A20">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B20">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D20">
         <v>5</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H20">
         <v>2</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L20">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B21">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C21">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D21">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F21">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H21">
         <v>2</v>
       </c>
       <c r="J21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L21">
         <v>1</v>
@@ -2284,25 +2284,25 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B22">
         <v>6</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D22">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F22">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J22">
         <v>0</v>
@@ -2313,28 +2313,28 @@
     </row>
     <row r="23" spans="1:12">
       <c r="A23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B23">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C23">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E23">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L23">
         <v>1</v>
@@ -2342,28 +2342,28 @@
     </row>
     <row r="24" spans="1:12">
       <c r="A24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B24">
         <v>4</v>
       </c>
       <c r="C24">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D24">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F24">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J24">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L24">
         <v>1</v>
@@ -2371,57 +2371,57 @@
     </row>
     <row r="25" spans="1:12">
       <c r="A25">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B25">
         <v>2</v>
       </c>
       <c r="C25">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D25">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F25">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L25">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:12">
       <c r="A26">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B26">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E26">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L26">
         <v>1</v>
@@ -2429,22 +2429,22 @@
     </row>
     <row r="27" spans="1:12">
       <c r="A27">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B27">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C27">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D27">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E27">
         <v>2</v>
       </c>
       <c r="F27">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H27">
         <v>3</v>
@@ -2458,22 +2458,22 @@
     </row>
     <row r="28" spans="1:12">
       <c r="A28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B28">
         <v>6</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D28">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E28">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F28">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H28">
         <v>3</v>
@@ -2487,28 +2487,28 @@
     </row>
     <row r="29" spans="1:12">
       <c r="A29">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B29">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C29">
         <v>3</v>
       </c>
       <c r="D29">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F29">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H29">
         <v>3</v>
       </c>
       <c r="J29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L29">
         <v>1</v>
@@ -2516,22 +2516,22 @@
     </row>
     <row r="30" spans="1:12">
       <c r="A30">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B30">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D30">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E30">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F30">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H30">
         <v>3</v>
@@ -2545,28 +2545,28 @@
     </row>
     <row r="31" spans="1:12">
       <c r="A31">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B31">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C31">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D31">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E31">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H31">
         <v>3</v>
       </c>
       <c r="J31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L31">
         <v>1</v>
@@ -2574,19 +2574,19 @@
     </row>
     <row r="32" spans="1:12">
       <c r="A32">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B32">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C32">
         <v>3</v>
       </c>
       <c r="D32">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E32">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -2603,28 +2603,28 @@
     </row>
     <row r="33" spans="1:12">
       <c r="A33">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B33">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D33">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E33">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F33">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H33">
         <v>3</v>
       </c>
       <c r="J33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L33">
         <v>1</v>
@@ -2632,28 +2632,28 @@
     </row>
     <row r="34" spans="1:12">
       <c r="A34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B34">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C34">
         <v>3</v>
       </c>
       <c r="D34">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E34">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F34">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H34">
         <v>3</v>
       </c>
       <c r="J34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L34">
         <v>1</v>
@@ -2661,28 +2661,28 @@
     </row>
     <row r="35" spans="1:12">
       <c r="A35">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B35">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C35">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D35">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E35">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F35">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H35">
         <v>3</v>
       </c>
       <c r="J35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L35">
         <v>1</v>
@@ -2690,25 +2690,25 @@
     </row>
     <row r="36" spans="1:12">
       <c r="A36">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B36">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C36">
         <v>6</v>
       </c>
       <c r="D36">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E36">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F36">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H36">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J36">
         <v>0</v>
@@ -2719,28 +2719,28 @@
     </row>
     <row r="37" spans="1:12">
       <c r="A37">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C37">
         <v>3</v>
       </c>
       <c r="D37">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E37">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H37">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L37">
         <v>1</v>
@@ -2748,28 +2748,28 @@
     </row>
     <row r="38" spans="1:12">
       <c r="A38">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B38">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C38">
         <v>3</v>
       </c>
       <c r="D38">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E38">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F38">
         <v>2</v>
       </c>
       <c r="H38">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L38">
         <v>1</v>
@@ -2777,28 +2777,28 @@
     </row>
     <row r="39" spans="1:12">
       <c r="A39">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B39">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D39">
         <v>5</v>
       </c>
       <c r="E39">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H39">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L39">
         <v>1</v>
@@ -2806,28 +2806,28 @@
     </row>
     <row r="40" spans="1:12">
       <c r="A40">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B40">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C40">
         <v>4</v>
       </c>
       <c r="D40">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E40">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F40">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H40">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L40">
         <v>1</v>
@@ -2835,28 +2835,28 @@
     </row>
     <row r="41" spans="1:12">
       <c r="A41">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B41">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C41">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D41">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F41">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H41">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L41">
         <v>1</v>
@@ -2864,22 +2864,22 @@
     </row>
     <row r="42" spans="1:12">
       <c r="A42">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C42">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D42">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E42">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H42">
         <v>4</v>
@@ -2893,22 +2893,22 @@
     </row>
     <row r="43" spans="1:12">
       <c r="A43">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B43">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C43">
         <v>3</v>
       </c>
       <c r="D43">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E43">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H43">
         <v>4</v>
@@ -2922,28 +2922,28 @@
     </row>
     <row r="44" spans="1:12">
       <c r="A44">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B44">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C44">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D44">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E44">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F44">
         <v>1</v>
       </c>
       <c r="H44">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J44">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L44">
         <v>1</v>
@@ -2951,204 +2951,30 @@
     </row>
     <row r="45" spans="1:12">
       <c r="A45">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B45">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C45">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D45">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E45">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F45">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H45">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12">
-      <c r="A46">
-        <v>4</v>
-      </c>
-      <c r="B46">
-        <v>2</v>
-      </c>
-      <c r="C46">
-        <v>5</v>
-      </c>
-      <c r="D46">
-        <v>3</v>
-      </c>
-      <c r="E46">
-        <v>1</v>
-      </c>
-      <c r="F46">
-        <v>6</v>
-      </c>
-      <c r="H46">
-        <v>4</v>
-      </c>
-      <c r="J46">
-        <v>1</v>
-      </c>
-      <c r="L46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12">
-      <c r="A47">
-        <v>3</v>
-      </c>
-      <c r="B47">
-        <v>6</v>
-      </c>
-      <c r="C47">
-        <v>4</v>
-      </c>
-      <c r="D47">
-        <v>5</v>
-      </c>
-      <c r="E47">
-        <v>1</v>
-      </c>
-      <c r="F47">
-        <v>2</v>
-      </c>
-      <c r="H47">
-        <v>4</v>
-      </c>
-      <c r="J47">
-        <v>3</v>
-      </c>
-      <c r="L47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12">
-      <c r="A48">
-        <v>5</v>
-      </c>
-      <c r="B48">
-        <v>6</v>
-      </c>
-      <c r="C48">
-        <v>1</v>
-      </c>
-      <c r="D48">
-        <v>3</v>
-      </c>
-      <c r="E48">
-        <v>4</v>
-      </c>
-      <c r="F48">
-        <v>2</v>
-      </c>
-      <c r="H48">
-        <v>4</v>
-      </c>
-      <c r="J48">
-        <v>0</v>
-      </c>
-      <c r="L48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12">
-      <c r="A49">
-        <v>5</v>
-      </c>
-      <c r="B49">
-        <v>2</v>
-      </c>
-      <c r="C49">
-        <v>3</v>
-      </c>
-      <c r="D49">
-        <v>4</v>
-      </c>
-      <c r="E49">
-        <v>1</v>
-      </c>
-      <c r="F49">
-        <v>6</v>
-      </c>
-      <c r="H49">
-        <v>4</v>
-      </c>
-      <c r="J49">
-        <v>1</v>
-      </c>
-      <c r="L49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12">
-      <c r="A50">
-        <v>2</v>
-      </c>
-      <c r="B50">
-        <v>1</v>
-      </c>
-      <c r="C50">
-        <v>4</v>
-      </c>
-      <c r="D50">
-        <v>3</v>
-      </c>
-      <c r="E50">
-        <v>6</v>
-      </c>
-      <c r="F50">
-        <v>5</v>
-      </c>
-      <c r="H50">
-        <v>5</v>
-      </c>
-      <c r="J50">
-        <v>1</v>
-      </c>
-      <c r="L50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12">
-      <c r="A51">
-        <v>5</v>
-      </c>
-      <c r="B51">
-        <v>1</v>
-      </c>
-      <c r="C51">
-        <v>4</v>
-      </c>
-      <c r="D51">
-        <v>3</v>
-      </c>
-      <c r="E51">
-        <v>6</v>
-      </c>
-      <c r="F51">
-        <v>2</v>
-      </c>
-      <c r="H51">
-        <v>5</v>
-      </c>
-      <c r="J51">
-        <v>1</v>
-      </c>
-      <c r="L51">
         <v>1</v>
       </c>
     </row>

</xml_diff>